<commit_message>
add new person in insert from, new function for edit inside web
</commit_message>
<xml_diff>
--- a/data/history.xlsx
+++ b/data/history.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
   <si>
     <t>id</t>
   </si>
@@ -77,6 +77,45 @@
   </si>
   <si>
     <t>07-05-2018 19:08</t>
+  </si>
+  <si>
+    <t>ten cty</t>
+  </si>
+  <si>
+    <t>23-05-2018 17:04</t>
+  </si>
+  <si>
+    <t>23-05-2018 17:05</t>
+  </si>
+  <si>
+    <t>to_call</t>
+  </si>
+  <si>
+    <t>23-05-2018 17:07</t>
+  </si>
+  <si>
+    <t>23-05-2018 17:11</t>
+  </si>
+  <si>
+    <t>23-05-2018 17:12</t>
+  </si>
+  <si>
+    <t>23-05-2018 17:13</t>
+  </si>
+  <si>
+    <t>23-05-2018 17:14</t>
+  </si>
+  <si>
+    <t>23-05-2018 17:15</t>
+  </si>
+  <si>
+    <t>23-05-2018 17:16</t>
+  </si>
+  <si>
+    <t>23-05-2018 17:17</t>
+  </si>
+  <si>
+    <t>23-05-2018 17:18</t>
   </si>
 </sst>
 </file>
@@ -390,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD9"/>
@@ -642,11 +681,701 @@
       <c r="E10" t="s">
         <v>20</v>
       </c>
-      <c r="F10" t="s"/>
       <c r="G10" t="b">
         <v>1</v>
       </c>
       <c r="H10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>11</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>11</v>
+      </c>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>31</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>11</v>
+      </c>
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G32" t="b">
+        <v>0</v>
+      </c>
+      <c r="H32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>11</v>
+      </c>
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>32</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>11</v>
+      </c>
+      <c r="C34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s">
+        <v>32</v>
+      </c>
+      <c r="G35" t="b">
+        <v>0</v>
+      </c>
+      <c r="H35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>11</v>
+      </c>
+      <c r="C36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" t="s">
+        <v>32</v>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>11</v>
+      </c>
+      <c r="C37" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" t="s">
+        <v>32</v>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>11</v>
+      </c>
+      <c r="C38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" t="s">
+        <v>32</v>
+      </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>11</v>
+      </c>
+      <c r="C39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" t="s">
+        <v>33</v>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>11</v>
+      </c>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" t="s"/>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>